<commit_message>
iniciando a tabela de clientes
</commit_message>
<xml_diff>
--- a/data/data_transformation.xlsx
+++ b/data/data_transformation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapos\Documents\PATRICK\PROJETOS\PYTHON PROJETOS\projeto_criar_DnD_dataset\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapos\Documents\PATRICK\PROJETOS\PYTHON PROJETOS\projeto_baldursgate_vendor_sales\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA5771F-C286-4070-94E4-D17CE652BC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5C6F80-C55C-4867-9108-29690DA7E42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-45" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-45" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="656">
   <si>
     <t>Name</t>
   </si>
@@ -1515,6 +1515,486 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Markus  Wintermere</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talfen  Daargen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tavon  Coyle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Malfier  Targana</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tegan  Drakantal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Namen  Redraven</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dodd  Falck</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talfen  Hindergrass</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fenton  Redraven</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vanan  Varcona</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Leyten  Ronefel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dalkon  Swiller</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talfen  Wintermere</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vincent  Cresthill</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cale  Zereni</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talfen  Caskajaro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cale  Ramcrown</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Norris  Irongull</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sevenson  Lamoth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hagar  Zereni</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Taran  Drakantal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eandro  Coyle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Falken  Armanci</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bram  Ereghast</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Falken  Daargen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arando Arkalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jeras  Dalicarlia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talfen  Fallenbridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Steveren  Ramcrown</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tavon  Silvergraft</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dodd  Zereni</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gryphero  Webb</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fenton  Varzand</t>
+  </si>
+  <si>
+    <t>Anlow  Ereghast</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quentin  Coyle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hagar  Pyncion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Krynt  Lamoth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talfen  Swiller</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nerle  Daargen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ningyan  Daargen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Norris  Seratolva</t>
+  </si>
+  <si>
+    <t>Beyla  Lamoth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zebel  Ereghast</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grenenzel  Copperhearth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Xandrilla  Pyncion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Velene  Hackshield</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lyfalia  Ayrthwil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thirya  Grantham</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marnia  Vrye</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lurka  Bilger</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sachil  Webb</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zebel  Van Gandt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Velene Ambershard</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rokel  Fryft</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sachil  Cresthill</t>
+  </si>
+  <si>
+    <t>Aryllan  Zethergyll</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Remora  Hackshield</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Krystolari  Wilxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Remora  Welfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lyfalia  Varzand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thirya  Dalicarlia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Xandrilla  Grantham</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Xandrilla  Falck</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Irva  Hindergrass</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zebel  Lamoth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tura Ambershard</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vencia  Zethergyll</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vencia  Cresthill</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hallan  Copperhearth</t>
+  </si>
+  <si>
+    <t>Azura  Graylock</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Irva  Grimtor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Veklani  Varzand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tylsa  Webb</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vronwe  Cuttlescar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brey  Graylock</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sachil  Velene</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lorelei  Revenmar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ronefel  Towerfall</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rosalyn  Rockharvest</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Roksana  Coyle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rosalyn  Van Gandt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ronefel  Venefiq</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marnia  Leerstrom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Venefiq  Barrelhelm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Remora  Moonridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ronefel  Wygarthe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grenenzel  Welfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Krystolari  Roxley</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thurlfara  Evermead</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hallan  Fletcher</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mirabel  Zereni</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zebel  Cuttlescar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zebel  Zatchet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fenryl  Leerstrom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Praxana  Lynchfield</t>
+  </si>
+  <si>
+    <t>Azura  Evermead</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mirabel  Caskajaro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brey  Fallenbridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marnia  Grimtor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Venefiq  Vrye</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ronefel  Welfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grenenzel  Varzand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Praxana  Strong</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Venefiq  Revenmar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thurlfara  Ratley</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marnia  Oakenheart</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hallan  Shanks</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thurlfara Aryllan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lyfalia  Hindergrass</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vronwe  Carnavon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marnia  Blackstrand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Saidi  Ereghast</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Krystolari  Silvertarn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mirabel  Zethergyll</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marnia  Roxley</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Irva  Velene</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mirabel  Irongull</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lokara  Iscalon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thurlfara  Leerstrom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lorelei  Umbermoor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mirabel Aryllan</t>
+  </si>
+  <si>
+    <t>Azura  Netheridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Remora  Atalya</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hallan  Hackshield</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fenryl  Venefiq</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pharana  Zarkanan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Venefiq  Varzand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brey  Coldshore</t>
+  </si>
+  <si>
+    <t>Azura  Stormchapel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Irva Aryllan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Saidi  Shattermast</t>
+  </si>
+  <si>
+    <t>Aryllan  Sell</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tanika Ambershard</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ronefel  Graylock</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fenryl  Netheridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vronwe  Blackstrand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ronefel  Dunhall</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tanika  Shanks</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lurka  Swiller</t>
+  </si>
+  <si>
+    <t>Aryllan  Leerstrom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hallan  Zethergyll</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fenryl  Irva</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tylsa  Kreel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tanika  Wygarthe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grenenzel  Deepmiddens</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pharana  Dunhall</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grenenzel  Coldshore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ronefel  Ratley</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brey Aryllan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ronefel  Stormchapel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kasaki  Talandro </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Venefiq  Ereghast</t>
+  </si>
+  <si>
+    <t>Beyla  Revenmar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Roksana  Dalicarlia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lyfalia  Wintermere</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brey  Danamark</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Remora  Lamoth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ronefel  Irva</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sachil  Redraven</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pharana  Skandalor</t>
   </si>
 </sst>
 </file>
@@ -2617,8 +3097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB456DC9-6855-485E-B473-18133F10468F}">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2668,19 +3148,19 @@
       </c>
       <c r="D2" t="str">
         <f ca="1">INDEX($A$2:$A$41,F2,1)&amp;" "&amp;INDEX($C$2:$C$97,G2,1)</f>
-        <v xml:space="preserve"> Vanan  Oakenheart</v>
+        <v xml:space="preserve"> Ningyan  Fletcher</v>
       </c>
       <c r="E2" t="str">
         <f ca="1">INDEX($B$2:$B$42,F2,1)&amp;" "&amp;INDEX($C$2:$C$97,G2,1)</f>
-        <v xml:space="preserve"> Velene  Oakenheart</v>
+        <v xml:space="preserve"> Vauldra  Fletcher</v>
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1,ROW($A$40))</f>
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="G2">
         <f ca="1">RANDBETWEEN(1,ROW($C$96))</f>
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
         <v>281</v>
@@ -2700,20 +3180,20 @@
         <v>167</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D66" ca="1" si="0">INDEX($A$2:$A$41,F3,1)&amp;" "&amp;INDEX($C$2:$C$97,G3,1)</f>
-        <v xml:space="preserve"> Markus  Netheridge</v>
+        <f t="shared" ref="D3:D42" ca="1" si="0">INDEX($A$2:$A$41,F3,1)&amp;" "&amp;INDEX($C$2:$C$97,G3,1)</f>
+        <v xml:space="preserve"> Feck  Silvergraft</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" ca="1" si="1">INDEX($B$2:$B$42,F3,1)&amp;" "&amp;INDEX($C$2:$C$97,G3,1)</f>
-        <v xml:space="preserve"> Lurka  Netheridge</v>
+        <f t="shared" ref="E3:E42" ca="1" si="1">INDEX($B$2:$B$42,F3,1)&amp;" "&amp;INDEX($C$2:$C$97,G3,1)</f>
+        <v xml:space="preserve"> Tanika  Silvergraft</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F42" ca="1" si="2">RANDBETWEEN(1,ROW($A$40))</f>
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G66" ca="1" si="3">RANDBETWEEN(1,ROW($C$96))</f>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="H3" s="1">
         <f>PRODUCT(COUNTA(A2:A41),COUNTA(C2:C97))</f>
@@ -2736,19 +3216,19 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Dodd  Fryft</v>
+        <v xml:space="preserve"> Arando  Varzand</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Pharana  Fryft</v>
+        <v xml:space="preserve"> Brey  Varzand</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2763,19 +3243,19 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Vincent  Vrye</v>
+        <v xml:space="preserve"> Dodd  Rockharvest</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Venefiq  Vrye</v>
+        <v xml:space="preserve"> Pharana  Rockharvest</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="2"/>
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="3"/>
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2790,19 +3270,19 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Krynt  Silvertarn</v>
+        <v xml:space="preserve"> Leyten  Ereghast</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Beyla  Silvertarn</v>
+        <v xml:space="preserve"> Grenenzel  Ereghast</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="3"/>
-        <v>84</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2817,19 +3297,19 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Falken  Armanci</v>
+        <v xml:space="preserve"> Tamond  Wygarthe</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Saidi  Armanci</v>
+        <v xml:space="preserve"> Irva  Wygarthe</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2844,11 +3324,11 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Jeras  Redraven</v>
+        <v xml:space="preserve"> Jeras  Umbermoor</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Xandrilla  Redraven</v>
+        <v xml:space="preserve"> Xandrilla  Umbermoor</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="2"/>
@@ -2856,7 +3336,7 @@
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="3"/>
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2871,19 +3351,19 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Nilus  Fryft</v>
+        <v xml:space="preserve"> Lavant  Barrelhelm</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Thurlfara  Fryft</v>
+        <v xml:space="preserve"> Fenryl  Barrelhelm</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2898,19 +3378,19 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Tavon  Drakantal</v>
+        <v xml:space="preserve"> Navaren  Van Devries</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Ronefel  Drakantal</v>
+        <v xml:space="preserve"> Rokel  Van Devries</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="2"/>
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="3"/>
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2925,19 +3405,19 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Semil  Lyfalia</v>
+        <v xml:space="preserve"> Arando  Carnavon</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Zebel  Lyfalia</v>
+        <v xml:space="preserve"> Brey  Carnavon</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="2"/>
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="3"/>
-        <v>91</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2952,19 +3432,19 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Lavant  Daargen</v>
+        <v xml:space="preserve"> Taran  Cuttlescar</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Fenryl  Daargen</v>
+        <v xml:space="preserve"> Lyfalia  Cuttlescar</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="3"/>
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2979,19 +3459,19 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Vanan  Talandro </v>
+        <v xml:space="preserve"> Semil  Moonridge</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Velene  Talandro </v>
+        <v xml:space="preserve"> Zebel  Moonridge</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="2"/>
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="3"/>
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3006,19 +3486,19 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Dyrk  Kroft</v>
+        <v xml:space="preserve"> Krynt  Van Gandt</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Rosalyn  Kroft</v>
+        <v>Beyla  Van Gandt</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3033,19 +3513,19 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Dalkon  Van Gandt</v>
+        <v xml:space="preserve"> Dungarth  Drakantal</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Lorelei  Van Gandt</v>
+        <v xml:space="preserve"> Remora  Drakantal</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="3"/>
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3060,19 +3540,19 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Jeras  Bilger</v>
+        <v xml:space="preserve"> Ningyan  Stavenger</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Xandrilla  Bilger</v>
+        <v xml:space="preserve"> Vauldra  Stavenger</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -3087,19 +3567,19 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Meklan  Iscalon</v>
+        <v xml:space="preserve"> Semil  Atalya</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Marnia  Iscalon</v>
+        <f ca="1">INDEX($B$2:$B$42,F17,1)&amp;" "&amp;INDEX($C$2:$C$97,G17,1)</f>
+        <v xml:space="preserve"> Zebel  Atalya</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="3"/>
-        <v>29</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3114,19 +3594,19 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Semil Arkalis</v>
+        <v xml:space="preserve"> Leyten  Zereni</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Zebel Arkalis</v>
+        <v xml:space="preserve"> Grenenzel  Zereni</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="2"/>
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -3141,19 +3621,19 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Falken  Danamark</v>
+        <v xml:space="preserve"> Dalkon  Drakantal</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Saidi  Danamark</v>
+        <v xml:space="preserve"> Lorelei  Drakantal</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -3168,19 +3648,19 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Nerle  Coyle</v>
+        <v xml:space="preserve"> Falken  Umbermoor</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Roksana  Coyle</v>
+        <v xml:space="preserve"> Saidi  Umbermoor</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -3195,19 +3675,19 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Norris  Goldrudder</v>
+        <v xml:space="preserve"> Dyrk  Grantham</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Veklani  Goldrudder</v>
+        <v xml:space="preserve"> Rosalyn  Grantham</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -3222,19 +3702,19 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Semil  Fletcher</v>
+        <v xml:space="preserve"> Steveren  Atalya</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Zebel  Fletcher</v>
+        <v xml:space="preserve"> Atalya  Atalya</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="2"/>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="3"/>
-        <v>22</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -3249,19 +3729,19 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Nilus  Ereghast</v>
+        <v xml:space="preserve"> Sevenson  Fallenbridge</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Thurlfara  Ereghast</v>
+        <v>Aryllan  Fallenbridge</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="3"/>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -3276,19 +3756,19 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Taran  Lyfalia</v>
+        <v xml:space="preserve"> Krynt  Swiller</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Lyfalia  Lyfalia</v>
+        <v>Beyla  Swiller</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="2"/>
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="3"/>
-        <v>91</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -3303,19 +3783,19 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Dalkon  Pyncion</v>
+        <v xml:space="preserve"> Krynt  Thirya</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Lorelei  Pyncion</v>
+        <v>Beyla  Thirya</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -3330,19 +3810,19 @@
       </c>
       <c r="D26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Malfier  Swiller</v>
+        <v xml:space="preserve"> Vanan  Cresthill</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Lokara  Swiller</v>
+        <v xml:space="preserve"> Velene  Cresthill</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="3"/>
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -3357,19 +3837,19 @@
       </c>
       <c r="D27" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Daylen  Danamark</v>
+        <v xml:space="preserve"> Taran  Kreel</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Mirabel  Danamark</v>
+        <v xml:space="preserve"> Lyfalia  Kreel</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3384,19 +3864,19 @@
       </c>
       <c r="D28" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Norris  Umbermoor</v>
+        <v xml:space="preserve"> Daylen  Wintermere</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Veklani  Umbermoor</v>
+        <v xml:space="preserve"> Mirabel  Wintermere</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="3"/>
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -3411,19 +3891,19 @@
       </c>
       <c r="D29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Madian  Shanks</v>
+        <v xml:space="preserve"> Lavant  Oakenheart</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Krystolari  Shanks</v>
+        <v xml:space="preserve"> Fenryl  Oakenheart</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="3"/>
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3438,19 +3918,19 @@
       </c>
       <c r="D30" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Quentin  Irva</v>
+        <v xml:space="preserve"> Steveren  Gullscream</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Vronwe  Irva</v>
+        <v xml:space="preserve"> Atalya  Gullscream</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="3"/>
-        <v>90</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -3465,19 +3945,19 @@
       </c>
       <c r="D31" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Falken Aryllan</v>
+        <v xml:space="preserve"> Cale  Oakenheart</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Saidi Aryllan</v>
+        <v xml:space="preserve"> Kasaki  Oakenheart</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="3"/>
-        <v>87</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3492,19 +3972,19 @@
       </c>
       <c r="D32" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Taran  Coldshore</v>
+        <v xml:space="preserve"> Tavon Arkalis</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Lyfalia  Coldshore</v>
+        <v xml:space="preserve"> Ronefel Arkalis</v>
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="2"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -3519,19 +3999,19 @@
       </c>
       <c r="D33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Eandro  Targana</v>
+        <v xml:space="preserve"> Bram  Blackstrand</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Sachil  Targana</v>
+        <v xml:space="preserve"> Hallan  Blackstrand</v>
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="3"/>
-        <v>54</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -3546,11 +4026,11 @@
       </c>
       <c r="D34" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Vanan  Fryft</v>
+        <v xml:space="preserve"> Vanan  Markolak</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Velene  Fryft</v>
+        <v xml:space="preserve"> Velene  Markolak</v>
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="2"/>
@@ -3558,7 +4038,7 @@
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3573,19 +4053,19 @@
       </c>
       <c r="D35" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Vanan  Hindergrass</v>
+        <v xml:space="preserve"> Leyten  Graylock</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Velene  Hindergrass</v>
+        <v xml:space="preserve"> Grenenzel  Graylock</v>
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="2"/>
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3600,19 +4080,19 @@
       </c>
       <c r="D36" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Ningyan  Skandalor</v>
+        <v xml:space="preserve"> Lavant  Pyncion</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Vauldra  Skandalor</v>
+        <v xml:space="preserve"> Fenryl  Pyncion</v>
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="3"/>
-        <v>85</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3627,19 +4107,19 @@
       </c>
       <c r="D37" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Daylen  Leerstrom</v>
+        <v xml:space="preserve"> Namen  Drakantal</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Mirabel  Leerstrom</v>
+        <v xml:space="preserve"> Praxana  Drakantal</v>
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="G37">
         <f t="shared" ca="1" si="3"/>
-        <v>33</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3654,19 +4134,19 @@
       </c>
       <c r="D38" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Steveren  Venefiq</v>
+        <v xml:space="preserve"> Dyrk  Daargen</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Atalya  Venefiq</v>
+        <v xml:space="preserve"> Rosalyn  Daargen</v>
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="2"/>
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="G38">
         <f t="shared" ca="1" si="3"/>
-        <v>95</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3681,19 +4161,19 @@
       </c>
       <c r="D39" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Bram  Targana</v>
+        <v xml:space="preserve"> Nerle  Roxley</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Hallan  Targana</v>
+        <v xml:space="preserve"> Roksana  Roxley</v>
       </c>
       <c r="F39">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="G39">
         <f t="shared" ca="1" si="3"/>
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3708,19 +4188,19 @@
       </c>
       <c r="D40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Jeras  Rockharvest</v>
+        <v xml:space="preserve"> Hagar  Fallenbridge</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Xandrilla  Rockharvest</v>
+        <v xml:space="preserve"> Vencia  Fallenbridge</v>
       </c>
       <c r="F40">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G40">
         <f t="shared" ca="1" si="3"/>
-        <v>83</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3735,19 +4215,19 @@
       </c>
       <c r="D41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Madian  Daargen</v>
+        <v xml:space="preserve"> Markus  Hackshield</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Krystolari  Daargen</v>
+        <v xml:space="preserve"> Lurka  Hackshield</v>
       </c>
       <c r="F41">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G41">
         <f t="shared" ca="1" si="3"/>
-        <v>12</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3759,19 +4239,19 @@
       </c>
       <c r="D42" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve"> Nerle  Webb</v>
+        <v xml:space="preserve"> Jeras  Ayrthwil</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve"> Roksana  Webb</v>
+        <v xml:space="preserve"> Xandrilla  Ayrthwil</v>
       </c>
       <c r="F42">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G42">
         <f t="shared" ca="1" si="3"/>
-        <v>64</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3780,7 +4260,7 @@
       </c>
       <c r="G43">
         <f t="shared" ca="1" si="3"/>
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3789,7 +4269,7 @@
       </c>
       <c r="G44">
         <f t="shared" ca="1" si="3"/>
-        <v>84</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3798,7 +4278,7 @@
       </c>
       <c r="G45">
         <f t="shared" ca="1" si="3"/>
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3807,7 +4287,7 @@
       </c>
       <c r="G46">
         <f t="shared" ca="1" si="3"/>
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3816,7 +4296,7 @@
       </c>
       <c r="G47">
         <f t="shared" ca="1" si="3"/>
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3825,7 +4305,7 @@
       </c>
       <c r="G48">
         <f t="shared" ca="1" si="3"/>
-        <v>58</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">
@@ -3834,7 +4314,7 @@
       </c>
       <c r="G49">
         <f t="shared" ca="1" si="3"/>
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.25">
@@ -3843,7 +4323,7 @@
       </c>
       <c r="G50">
         <f t="shared" ca="1" si="3"/>
-        <v>43</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.25">
@@ -3852,7 +4332,7 @@
       </c>
       <c r="G51">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
@@ -3861,7 +4341,7 @@
       </c>
       <c r="G52">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.25">
@@ -3870,7 +4350,7 @@
       </c>
       <c r="G53">
         <f t="shared" ca="1" si="3"/>
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.25">
@@ -3879,7 +4359,7 @@
       </c>
       <c r="G54">
         <f t="shared" ca="1" si="3"/>
-        <v>45</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.25">
@@ -3888,7 +4368,7 @@
       </c>
       <c r="G55">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.25">
@@ -3897,7 +4377,7 @@
       </c>
       <c r="G56">
         <f t="shared" ca="1" si="3"/>
-        <v>65</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.25">
@@ -3906,7 +4386,7 @@
       </c>
       <c r="G57">
         <f t="shared" ca="1" si="3"/>
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.25">
@@ -3915,7 +4395,7 @@
       </c>
       <c r="G58">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.25">
@@ -3924,7 +4404,7 @@
       </c>
       <c r="G59">
         <f t="shared" ca="1" si="3"/>
-        <v>69</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.25">
@@ -3933,7 +4413,7 @@
       </c>
       <c r="G60">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.25">
@@ -3942,7 +4422,7 @@
       </c>
       <c r="G61">
         <f t="shared" ca="1" si="3"/>
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
@@ -3951,7 +4431,7 @@
       </c>
       <c r="G62">
         <f t="shared" ca="1" si="3"/>
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
@@ -3960,7 +4440,7 @@
       </c>
       <c r="G63">
         <f t="shared" ca="1" si="3"/>
-        <v>46</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.25">
@@ -3969,7 +4449,7 @@
       </c>
       <c r="G64">
         <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
@@ -3978,7 +4458,7 @@
       </c>
       <c r="G65">
         <f t="shared" ca="1" si="3"/>
-        <v>79</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
@@ -3987,7 +4467,7 @@
       </c>
       <c r="G66">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.25">
@@ -3996,7 +4476,7 @@
       </c>
       <c r="G67">
         <f t="shared" ref="G67:G97" ca="1" si="4">RANDBETWEEN(1,ROW($C$96))</f>
-        <v>7</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.25">
@@ -4005,7 +4485,7 @@
       </c>
       <c r="G68">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
@@ -4014,7 +4494,7 @@
       </c>
       <c r="G69">
         <f t="shared" ca="1" si="4"/>
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.25">
@@ -4023,7 +4503,7 @@
       </c>
       <c r="G70">
         <f t="shared" ca="1" si="4"/>
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.25">
@@ -4032,7 +4512,7 @@
       </c>
       <c r="G71">
         <f t="shared" ca="1" si="4"/>
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.25">
@@ -4041,7 +4521,7 @@
       </c>
       <c r="G72">
         <f t="shared" ca="1" si="4"/>
-        <v>29</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.25">
@@ -4050,7 +4530,7 @@
       </c>
       <c r="G73">
         <f t="shared" ca="1" si="4"/>
-        <v>80</v>
+        <v>52</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.25">
@@ -4059,7 +4539,7 @@
       </c>
       <c r="G74">
         <f t="shared" ca="1" si="4"/>
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.25">
@@ -4068,7 +4548,7 @@
       </c>
       <c r="G75">
         <f t="shared" ca="1" si="4"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.25">
@@ -4077,7 +4557,7 @@
       </c>
       <c r="G76">
         <f t="shared" ca="1" si="4"/>
-        <v>47</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.25">
@@ -4086,7 +4566,7 @@
       </c>
       <c r="G77">
         <f t="shared" ca="1" si="4"/>
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.25">
@@ -4095,7 +4575,7 @@
       </c>
       <c r="G78">
         <f t="shared" ca="1" si="4"/>
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.25">
@@ -4104,7 +4584,7 @@
       </c>
       <c r="G79">
         <f t="shared" ca="1" si="4"/>
-        <v>66</v>
+        <v>87</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.25">
@@ -4113,7 +4593,7 @@
       </c>
       <c r="G80">
         <f t="shared" ca="1" si="4"/>
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.25">
@@ -4122,7 +4602,7 @@
       </c>
       <c r="G81">
         <f t="shared" ca="1" si="4"/>
-        <v>36</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.25">
@@ -4131,7 +4611,7 @@
       </c>
       <c r="G82">
         <f t="shared" ca="1" si="4"/>
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.25">
@@ -4140,7 +4620,7 @@
       </c>
       <c r="G83">
         <f t="shared" ca="1" si="4"/>
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
     <row r="84" spans="3:7" x14ac:dyDescent="0.25">
@@ -4149,7 +4629,7 @@
       </c>
       <c r="G84">
         <f t="shared" ca="1" si="4"/>
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="3:7" x14ac:dyDescent="0.25">
@@ -4158,7 +4638,7 @@
       </c>
       <c r="G85">
         <f t="shared" ca="1" si="4"/>
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.25">
@@ -4167,7 +4647,7 @@
       </c>
       <c r="G86">
         <f t="shared" ca="1" si="4"/>
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.25">
@@ -4176,7 +4656,7 @@
       </c>
       <c r="G87">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>67</v>
       </c>
     </row>
     <row r="88" spans="3:7" x14ac:dyDescent="0.25">
@@ -4185,7 +4665,7 @@
       </c>
       <c r="G88">
         <f t="shared" ca="1" si="4"/>
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.25">
@@ -4194,7 +4674,7 @@
       </c>
       <c r="G89">
         <f t="shared" ca="1" si="4"/>
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.25">
@@ -4203,7 +4683,7 @@
       </c>
       <c r="G90">
         <f t="shared" ca="1" si="4"/>
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.25">
@@ -4212,7 +4692,7 @@
       </c>
       <c r="G91">
         <f t="shared" ca="1" si="4"/>
-        <v>20</v>
+        <v>75</v>
       </c>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.25">
@@ -4221,7 +4701,7 @@
       </c>
       <c r="G92">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93" spans="3:7" x14ac:dyDescent="0.25">
@@ -4230,7 +4710,7 @@
       </c>
       <c r="G93">
         <f t="shared" ca="1" si="4"/>
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.25">
@@ -4239,7 +4719,7 @@
       </c>
       <c r="G94">
         <f t="shared" ca="1" si="4"/>
-        <v>91</v>
+        <v>42</v>
       </c>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.25">
@@ -4248,7 +4728,7 @@
       </c>
       <c r="G95">
         <f t="shared" ca="1" si="4"/>
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.25">
@@ -4266,7 +4746,7 @@
       </c>
       <c r="G97">
         <f t="shared" ca="1" si="4"/>
-        <v>82</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -4276,13 +4756,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E57C30F-A484-4CFB-B9A6-BD0C0B1F4879}">
-  <dimension ref="A1:B206"/>
+  <dimension ref="A1:B411"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A393" workbookViewId="0">
+      <selection activeCell="A411" sqref="A411"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5934,6 +6416,1646 @@
         <v>494</v>
       </c>
     </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>496</v>
+      </c>
+      <c r="B207" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>497</v>
+      </c>
+      <c r="B208" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>498</v>
+      </c>
+      <c r="B209" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>499</v>
+      </c>
+      <c r="B210" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>500</v>
+      </c>
+      <c r="B211" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>501</v>
+      </c>
+      <c r="B212" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>502</v>
+      </c>
+      <c r="B213" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>503</v>
+      </c>
+      <c r="B214" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>504</v>
+      </c>
+      <c r="B215" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>505</v>
+      </c>
+      <c r="B216" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>506</v>
+      </c>
+      <c r="B217" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>507</v>
+      </c>
+      <c r="B218" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>508</v>
+      </c>
+      <c r="B219" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>509</v>
+      </c>
+      <c r="B220" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>510</v>
+      </c>
+      <c r="B221" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>511</v>
+      </c>
+      <c r="B222" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>512</v>
+      </c>
+      <c r="B223" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>513</v>
+      </c>
+      <c r="B224" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>514</v>
+      </c>
+      <c r="B225" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>515</v>
+      </c>
+      <c r="B226" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>516</v>
+      </c>
+      <c r="B227" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>517</v>
+      </c>
+      <c r="B228" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>518</v>
+      </c>
+      <c r="B229" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>519</v>
+      </c>
+      <c r="B230" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>520</v>
+      </c>
+      <c r="B231" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>521</v>
+      </c>
+      <c r="B232" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>522</v>
+      </c>
+      <c r="B233" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>523</v>
+      </c>
+      <c r="B234" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>524</v>
+      </c>
+      <c r="B235" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>525</v>
+      </c>
+      <c r="B236" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>526</v>
+      </c>
+      <c r="B237" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>527</v>
+      </c>
+      <c r="B238" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>528</v>
+      </c>
+      <c r="B239" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>529</v>
+      </c>
+      <c r="B240" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>530</v>
+      </c>
+      <c r="B241" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>531</v>
+      </c>
+      <c r="B242" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>532</v>
+      </c>
+      <c r="B243" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>533</v>
+      </c>
+      <c r="B244" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>534</v>
+      </c>
+      <c r="B245" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>535</v>
+      </c>
+      <c r="B246" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>536</v>
+      </c>
+      <c r="B247" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>496</v>
+      </c>
+      <c r="B248" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>497</v>
+      </c>
+      <c r="B249" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>498</v>
+      </c>
+      <c r="B250" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>499</v>
+      </c>
+      <c r="B251" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>500</v>
+      </c>
+      <c r="B252" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>501</v>
+      </c>
+      <c r="B253" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>502</v>
+      </c>
+      <c r="B254" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>503</v>
+      </c>
+      <c r="B255" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>504</v>
+      </c>
+      <c r="B256" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>505</v>
+      </c>
+      <c r="B257" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>506</v>
+      </c>
+      <c r="B258" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>507</v>
+      </c>
+      <c r="B259" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>508</v>
+      </c>
+      <c r="B260" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>509</v>
+      </c>
+      <c r="B261" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>510</v>
+      </c>
+      <c r="B262" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>511</v>
+      </c>
+      <c r="B263" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>512</v>
+      </c>
+      <c r="B264" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>513</v>
+      </c>
+      <c r="B265" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>514</v>
+      </c>
+      <c r="B266" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>515</v>
+      </c>
+      <c r="B267" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>516</v>
+      </c>
+      <c r="B268" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>517</v>
+      </c>
+      <c r="B269" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>518</v>
+      </c>
+      <c r="B270" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>519</v>
+      </c>
+      <c r="B271" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>520</v>
+      </c>
+      <c r="B272" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>521</v>
+      </c>
+      <c r="B273" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>522</v>
+      </c>
+      <c r="B274" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>523</v>
+      </c>
+      <c r="B275" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>524</v>
+      </c>
+      <c r="B276" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>525</v>
+      </c>
+      <c r="B277" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>526</v>
+      </c>
+      <c r="B278" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>527</v>
+      </c>
+      <c r="B279" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>528</v>
+      </c>
+      <c r="B280" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>529</v>
+      </c>
+      <c r="B281" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>530</v>
+      </c>
+      <c r="B282" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>531</v>
+      </c>
+      <c r="B283" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>532</v>
+      </c>
+      <c r="B284" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>533</v>
+      </c>
+      <c r="B285" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>534</v>
+      </c>
+      <c r="B286" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>535</v>
+      </c>
+      <c r="B287" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>536</v>
+      </c>
+      <c r="B288" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>538</v>
+      </c>
+      <c r="B289" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>539</v>
+      </c>
+      <c r="B290" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>540</v>
+      </c>
+      <c r="B291" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>541</v>
+      </c>
+      <c r="B292" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>542</v>
+      </c>
+      <c r="B293" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>467</v>
+      </c>
+      <c r="B294" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>543</v>
+      </c>
+      <c r="B295" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>544</v>
+      </c>
+      <c r="B296" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>545</v>
+      </c>
+      <c r="B297" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>546</v>
+      </c>
+      <c r="B298" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>547</v>
+      </c>
+      <c r="B299" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>548</v>
+      </c>
+      <c r="B300" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>549</v>
+      </c>
+      <c r="B301" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>550</v>
+      </c>
+      <c r="B302" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>551</v>
+      </c>
+      <c r="B303" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>552</v>
+      </c>
+      <c r="B304" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>317</v>
+      </c>
+      <c r="B305" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>553</v>
+      </c>
+      <c r="B306" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>554</v>
+      </c>
+      <c r="B307" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>555</v>
+      </c>
+      <c r="B308" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>556</v>
+      </c>
+      <c r="B309" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>557</v>
+      </c>
+      <c r="B310" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>558</v>
+      </c>
+      <c r="B311" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>559</v>
+      </c>
+      <c r="B312" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>560</v>
+      </c>
+      <c r="B313" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>561</v>
+      </c>
+      <c r="B314" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>562</v>
+      </c>
+      <c r="B315" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>563</v>
+      </c>
+      <c r="B316" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>564</v>
+      </c>
+      <c r="B317" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>565</v>
+      </c>
+      <c r="B318" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>566</v>
+      </c>
+      <c r="B319" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>567</v>
+      </c>
+      <c r="B320" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>537</v>
+      </c>
+      <c r="B321" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>568</v>
+      </c>
+      <c r="B322" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>569</v>
+      </c>
+      <c r="B323" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>570</v>
+      </c>
+      <c r="B324" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>571</v>
+      </c>
+      <c r="B325" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>572</v>
+      </c>
+      <c r="B326" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>573</v>
+      </c>
+      <c r="B327" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>574</v>
+      </c>
+      <c r="B328" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>575</v>
+      </c>
+      <c r="B329" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>576</v>
+      </c>
+      <c r="B330" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>577</v>
+      </c>
+      <c r="B331" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>578</v>
+      </c>
+      <c r="B332" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>579</v>
+      </c>
+      <c r="B333" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>580</v>
+      </c>
+      <c r="B334" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>581</v>
+      </c>
+      <c r="B335" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>582</v>
+      </c>
+      <c r="B336" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>583</v>
+      </c>
+      <c r="B337" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>584</v>
+      </c>
+      <c r="B338" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>585</v>
+      </c>
+      <c r="B339" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>586</v>
+      </c>
+      <c r="B340" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>587</v>
+      </c>
+      <c r="B341" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>588</v>
+      </c>
+      <c r="B342" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>589</v>
+      </c>
+      <c r="B343" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>590</v>
+      </c>
+      <c r="B344" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>591</v>
+      </c>
+      <c r="B345" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>592</v>
+      </c>
+      <c r="B346" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>593</v>
+      </c>
+      <c r="B347" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>594</v>
+      </c>
+      <c r="B348" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>595</v>
+      </c>
+      <c r="B349" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>596</v>
+      </c>
+      <c r="B350" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>477</v>
+      </c>
+      <c r="B351" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>597</v>
+      </c>
+      <c r="B352" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>598</v>
+      </c>
+      <c r="B353" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>599</v>
+      </c>
+      <c r="B354" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>600</v>
+      </c>
+      <c r="B355" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>601</v>
+      </c>
+      <c r="B356" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>602</v>
+      </c>
+      <c r="B357" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>603</v>
+      </c>
+      <c r="B358" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>604</v>
+      </c>
+      <c r="B359" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>605</v>
+      </c>
+      <c r="B360" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>606</v>
+      </c>
+      <c r="B361" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>607</v>
+      </c>
+      <c r="B362" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>608</v>
+      </c>
+      <c r="B363" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>609</v>
+      </c>
+      <c r="B364" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>610</v>
+      </c>
+      <c r="B365" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>611</v>
+      </c>
+      <c r="B366" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>612</v>
+      </c>
+      <c r="B367" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>613</v>
+      </c>
+      <c r="B368" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>614</v>
+      </c>
+      <c r="B369" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>615</v>
+      </c>
+      <c r="B370" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>616</v>
+      </c>
+      <c r="B371" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>617</v>
+      </c>
+      <c r="B372" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>489</v>
+      </c>
+      <c r="B373" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>618</v>
+      </c>
+      <c r="B374" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>619</v>
+      </c>
+      <c r="B375" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>620</v>
+      </c>
+      <c r="B376" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>621</v>
+      </c>
+      <c r="B377" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>622</v>
+      </c>
+      <c r="B378" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>623</v>
+      </c>
+      <c r="B379" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>624</v>
+      </c>
+      <c r="B380" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>625</v>
+      </c>
+      <c r="B381" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>626</v>
+      </c>
+      <c r="B382" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>627</v>
+      </c>
+      <c r="B383" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>628</v>
+      </c>
+      <c r="B384" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>629</v>
+      </c>
+      <c r="B385" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>630</v>
+      </c>
+      <c r="B386" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>631</v>
+      </c>
+      <c r="B387" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>632</v>
+      </c>
+      <c r="B388" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>633</v>
+      </c>
+      <c r="B389" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>634</v>
+      </c>
+      <c r="B390" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>635</v>
+      </c>
+      <c r="B391" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>636</v>
+      </c>
+      <c r="B392" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>637</v>
+      </c>
+      <c r="B393" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>638</v>
+      </c>
+      <c r="B394" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>639</v>
+      </c>
+      <c r="B395" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>640</v>
+      </c>
+      <c r="B396" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>641</v>
+      </c>
+      <c r="B397" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>642</v>
+      </c>
+      <c r="B398" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>643</v>
+      </c>
+      <c r="B399" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>644</v>
+      </c>
+      <c r="B400" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>645</v>
+      </c>
+      <c r="B401" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>646</v>
+      </c>
+      <c r="B402" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>647</v>
+      </c>
+      <c r="B403" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>648</v>
+      </c>
+      <c r="B404" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>649</v>
+      </c>
+      <c r="B405" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>650</v>
+      </c>
+      <c r="B406" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>651</v>
+      </c>
+      <c r="B407" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>652</v>
+      </c>
+      <c r="B408" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>653</v>
+      </c>
+      <c r="B409" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>654</v>
+      </c>
+      <c r="B410" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>655</v>
+      </c>
+      <c r="B411" t="s">
+        <v>493</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>